<commit_message>
App is now writing maintenance log
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -2,32 +2,40 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dsmith\projects\system-info-scan\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="repair_notes" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId2"/>
+    <sheet name="new_inventory" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
-  <si>
-    <t>OS</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+  <si>
+    <t>ID#</t>
+  </si>
+  <si>
+    <t>OS Info</t>
+  </si>
+  <si>
+    <t>CPU Data</t>
   </si>
   <si>
     <t>RAM</t>
   </si>
   <si>
-    <t>IP address</t>
+    <t>IP Address</t>
   </si>
   <si>
     <t>Date</t>
@@ -36,13 +44,127 @@
     <t>Time</t>
   </si>
   <si>
-    <t>Processor</t>
-  </si>
-  <si>
-    <t>Workstation</t>
-  </si>
-  <si>
     <t>Location</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>8264CLM</t>
+  </si>
+  <si>
+    <t>Windows-10-10.0.18362-SP0</t>
+  </si>
+  <si>
+    <t>Intel(R) Core(TM) i5-7300U CPU @ 2.60GHz</t>
+  </si>
+  <si>
+    <t>8 GB</t>
+  </si>
+  <si>
+    <t>10.110.200.154</t>
+  </si>
+  <si>
+    <t>07-16-2020</t>
+  </si>
+  <si>
+    <t>14:42</t>
+  </si>
+  <si>
+    <t>14:50</t>
+  </si>
+  <si>
+    <t>15:18</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>Dan Smith</t>
+  </si>
+  <si>
+    <t>16:16</t>
+  </si>
+  <si>
+    <t>This is working fine</t>
+  </si>
+  <si>
+    <t>ID #</t>
+  </si>
+  <si>
+    <t>Active</t>
+  </si>
+  <si>
+    <t>MfgCode</t>
+  </si>
+  <si>
+    <t>Model#</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>SN#</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>LocCode</t>
+  </si>
+  <si>
+    <t>PurDate</t>
+  </si>
+  <si>
+    <t>DeptDiv</t>
+  </si>
+  <si>
+    <t>IDComm</t>
+  </si>
+  <si>
+    <t>UT Notes</t>
+  </si>
+  <si>
+    <t>Inventory Year</t>
+  </si>
+  <si>
+    <t>Inventory Month</t>
+  </si>
+  <si>
+    <t>LT/DT</t>
+  </si>
+  <si>
+    <t>ArcMap</t>
+  </si>
+  <si>
+    <t>ArcPro</t>
+  </si>
+  <si>
+    <t>AutoCAD</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>FoxIT Pro</t>
+  </si>
+  <si>
+    <t>Lucity Desktop</t>
+  </si>
+  <si>
+    <t>OfficePro</t>
+  </si>
+  <si>
+    <t>BlueBeam Perpetual or Open</t>
+  </si>
+  <si>
+    <t>Other Specialized Software</t>
   </si>
 </sst>
 </file>
@@ -58,12 +180,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,8 +206,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -360,42 +502,272 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H1"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="11.59765625" customWidth="1"/>
+    <col min="1" max="1" width="11.59765625" style="6" customWidth="1"/>
+    <col min="2" max="2" width="29.59765625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="37.19921875" style="6" customWidth="1"/>
+    <col min="4" max="4" width="9.06640625" style="6"/>
+    <col min="5" max="5" width="16" style="6" customWidth="1"/>
+    <col min="6" max="6" width="19.1328125" style="6" customWidth="1"/>
+    <col min="7" max="8" width="9.06640625" style="6"/>
+    <col min="9" max="9" width="16.06640625" style="6" customWidth="1"/>
+    <col min="10" max="16384" width="9.06640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A3" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AB1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:28" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z1" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB1" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
created bat file to fetch missing info
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -344,13 +344,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="6" width="11.5703125"/>
     <col customWidth="1" max="2" min="2" style="6" width="29.5703125"/>
@@ -832,6 +832,58 @@
       <c r="J10" t="inlineStr">
         <is>
           <t>Kevyn Gero</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>8264CLM</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Windows-10-10.0.19041-SP0</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>Intel(R) Core(TM) i5-7300U CPU @ 2.60GHz</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>8 GB</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>10.110.200.112</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>10-15-2020</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>09:37</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>My PC</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Dan</t>
         </is>
       </c>
     </row>
@@ -864,13 +916,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y9"/>
+  <dimension ref="A1:Y10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="5" min="5" width="20.85546875"/>
     <col customWidth="1" max="14" min="14" width="13.5703125"/>
@@ -1467,6 +1519,68 @@
         </is>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>8264CLM</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Dell</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>XPS 15</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>5555</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Home</t>
+        </is>
+      </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="X10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Y10" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed error with initial software defaulting to 1 without input
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="repair_notes" sheetId="1" state="visible" r:id="rId1"/>
@@ -51,29 +51,29 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -344,24 +344,24 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="6" width="11.5703125"/>
-    <col customWidth="1" max="2" min="2" style="6" width="29.5703125"/>
-    <col customWidth="1" max="3" min="3" style="6" width="37.140625"/>
-    <col customWidth="1" max="4" min="4" style="6" width="9"/>
-    <col customWidth="1" max="5" min="5" style="6" width="16"/>
-    <col customWidth="1" max="6" min="6" style="6" width="19.140625"/>
-    <col customWidth="1" max="8" min="7" style="6" width="9"/>
-    <col customWidth="1" max="9" min="9" style="6" width="16"/>
-    <col customWidth="1" max="10" min="10" style="6" width="9"/>
-    <col customWidth="1" max="16384" min="11" style="6" width="9"/>
+    <col width="11.5703125" customWidth="1" style="6" min="1" max="1"/>
+    <col width="29.5703125" customWidth="1" style="6" min="2" max="2"/>
+    <col width="37.140625" customWidth="1" style="6" min="3" max="3"/>
+    <col width="9" customWidth="1" style="6" min="4" max="4"/>
+    <col width="16" customWidth="1" style="6" min="5" max="5"/>
+    <col width="19.140625" customWidth="1" style="6" min="6" max="6"/>
+    <col width="9" customWidth="1" style="6" min="7" max="8"/>
+    <col width="16" customWidth="1" style="6" min="9" max="9"/>
+    <col width="9" customWidth="1" style="6" min="10" max="10"/>
+    <col width="9" customWidth="1" style="6" min="11" max="16384"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -416,7 +416,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="2">
+    <row r="2" ht="30" customHeight="1">
       <c r="A2" s="6" t="inlineStr">
         <is>
           <t>8264CLM</t>
@@ -453,7 +453,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="3">
+    <row r="3" ht="30" customHeight="1">
       <c r="A3" s="6" t="inlineStr">
         <is>
           <t>8264CLM</t>
@@ -490,7 +490,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="4">
+    <row r="4" ht="30" customHeight="1">
       <c r="A4" s="6" t="inlineStr">
         <is>
           <t>8264CLM</t>
@@ -537,7 +537,7 @@
         </is>
       </c>
     </row>
-    <row customHeight="1" ht="30" r="5">
+    <row r="5" ht="30" customHeight="1">
       <c r="A5" s="6" t="inlineStr">
         <is>
           <t>8264CLM</t>
@@ -887,8 +887,107 @@
         </is>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>LAPTOP-K9FQV11C</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Windows-10-10.0.19041-SP0</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>Intel(R) Core(TM) i5-7200U CPU @ 2.50GHz</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>16 GB</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>192.168.1.130</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>12-20-2020</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>08:39</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>home</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>This is my personal laptop</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>Dan</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LAPTOP-K9FQV11C</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Windows-10-10.0.19041-SP0</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>Intel(R) Core(TM) i5-7200U CPU @ 2.50GHz</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>16 GB</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>192.168.1.130</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>12-20-2020</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>09:08</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>PY_VAR1</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>PY_VAR0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -906,7 +1005,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -916,19 +1015,19 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y10"/>
+  <dimension ref="A1:Y13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col customWidth="1" max="5" min="5" width="20.85546875"/>
-    <col customWidth="1" max="14" min="14" width="13.5703125"/>
-    <col customWidth="1" max="15" min="15" width="15.7109375"/>
-    <col customWidth="1" max="24" min="24" width="11.85546875"/>
-    <col customWidth="1" max="25" min="25" width="18.7109375"/>
+    <col width="20.85546875" customWidth="1" min="5" max="5"/>
+    <col width="13.5703125" customWidth="1" min="14" max="14"/>
+    <col width="15.7109375" customWidth="1" min="15" max="15"/>
+    <col width="11.85546875" customWidth="1" min="24" max="24"/>
+    <col width="18.7109375" customWidth="1" min="25" max="25"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1581,7 +1680,137 @@
         </is>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>LAPTOP-K9FQV11C</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>PY_VAR0</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>PY_VAR1</t>
+        </is>
+      </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y11" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>LAPTOP-K9FQV11C</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>PY_VAR0</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>PY_VAR1</t>
+        </is>
+      </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y12" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>LAPTOP-K9FQV11C</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
+      <c r="E13" t="inlineStr"/>
+      <c r="F13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>PY_VAR0</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>PY_VAR1</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Wrote python code to launch powershell scripts, and fixed some of them. Added firefox script
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="2" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12645" windowWidth="22260" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="repair_notes" sheetId="1" state="visible" r:id="rId1"/>
@@ -51,29 +51,29 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="14" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -344,7 +344,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
@@ -352,16 +352,16 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col width="11.5703125" customWidth="1" style="6" min="1" max="1"/>
-    <col width="29.5703125" customWidth="1" style="6" min="2" max="2"/>
-    <col width="37.140625" customWidth="1" style="6" min="3" max="3"/>
-    <col width="9" customWidth="1" style="6" min="4" max="4"/>
-    <col width="16" customWidth="1" style="6" min="5" max="5"/>
-    <col width="19.140625" customWidth="1" style="6" min="6" max="6"/>
-    <col width="9" customWidth="1" style="6" min="7" max="8"/>
-    <col width="16" customWidth="1" style="6" min="9" max="9"/>
-    <col width="9" customWidth="1" style="6" min="10" max="10"/>
-    <col width="9" customWidth="1" style="6" min="11" max="16384"/>
+    <col customWidth="1" max="1" min="1" style="6" width="11.5703125"/>
+    <col customWidth="1" max="2" min="2" style="6" width="29.5703125"/>
+    <col customWidth="1" max="3" min="3" style="6" width="37.140625"/>
+    <col customWidth="1" max="4" min="4" style="6" width="9"/>
+    <col customWidth="1" max="5" min="5" style="6" width="16"/>
+    <col customWidth="1" max="6" min="6" style="6" width="19.140625"/>
+    <col customWidth="1" max="8" min="7" style="6" width="9"/>
+    <col customWidth="1" max="9" min="9" style="6" width="16"/>
+    <col customWidth="1" max="10" min="10" style="6" width="9"/>
+    <col customWidth="1" max="16384" min="11" style="6" width="9"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -416,7 +416,7 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="30" customHeight="1">
+    <row customHeight="1" ht="30" r="2">
       <c r="A2" s="6" t="inlineStr">
         <is>
           <t>8264CLM</t>
@@ -453,7 +453,7 @@
         </is>
       </c>
     </row>
-    <row r="3" ht="30" customHeight="1">
+    <row customHeight="1" ht="30" r="3">
       <c r="A3" s="6" t="inlineStr">
         <is>
           <t>8264CLM</t>
@@ -490,7 +490,7 @@
         </is>
       </c>
     </row>
-    <row r="4" ht="30" customHeight="1">
+    <row customHeight="1" ht="30" r="4">
       <c r="A4" s="6" t="inlineStr">
         <is>
           <t>8264CLM</t>
@@ -537,7 +537,7 @@
         </is>
       </c>
     </row>
-    <row r="5" ht="30" customHeight="1">
+    <row customHeight="1" ht="30" r="5">
       <c r="A5" s="6" t="inlineStr">
         <is>
           <t>8264CLM</t>
@@ -986,8 +986,60 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>7992CL</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Windows-10-10.0.19041-SP0</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Intel(R) Core(TM) i5-8600 CPU @ 3.10GHz</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>32 GB</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>10.1.3.53</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>08-24-2021</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>13:39</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>PY_VAR1</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>This is a test</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>PY_VAR0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -1005,7 +1057,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -1023,11 +1075,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20.85546875" customWidth="1" min="5" max="5"/>
-    <col width="13.5703125" customWidth="1" min="14" max="14"/>
-    <col width="15.7109375" customWidth="1" min="15" max="15"/>
-    <col width="11.85546875" customWidth="1" min="24" max="24"/>
-    <col width="18.7109375" customWidth="1" min="25" max="25"/>
+    <col customWidth="1" max="5" min="5" width="20.85546875"/>
+    <col customWidth="1" max="14" min="14" width="13.5703125"/>
+    <col customWidth="1" max="15" min="15" width="15.7109375"/>
+    <col customWidth="1" max="24" min="24" width="11.85546875"/>
+    <col customWidth="1" max="25" min="25" width="18.7109375"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1775,10 +1827,6 @@
           <t>Y</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
-      <c r="E13" t="inlineStr"/>
-      <c r="F13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
           <t>PY_VAR0</t>
@@ -1811,6 +1859,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added line for icon, didn't work, will circle back later
</commit_message>
<xml_diff>
--- a/log.xlsx
+++ b/log.xlsx
@@ -344,13 +344,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="1" min="1" style="6" width="11.5703125"/>
     <col customWidth="1" max="2" min="2" style="6" width="29.5703125"/>
@@ -1033,6 +1033,58 @@
         </is>
       </c>
       <c r="J14" t="inlineStr">
+        <is>
+          <t>PY_VAR0</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>7992CL</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Windows-10-10.0.19041-SP0</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Intel(R) Core(TM) i5-8600 CPU @ 3.10GHz</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>32 GB</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>10.1.3.53</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>08-24-2021</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>16:09</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>PY_VAR1</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>This is me writing in the log</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
         <is>
           <t>PY_VAR0</t>
         </is>
@@ -1067,13 +1119,13 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Y13"/>
+  <dimension ref="A1:Y14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
       <selection activeCell="Y1" sqref="Y1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col customWidth="1" max="5" min="5" width="20.85546875"/>
     <col customWidth="1" max="14" min="14" width="13.5703125"/>
@@ -1858,6 +1910,68 @@
         </is>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>7992CL</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>Dell</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Optiplex</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>Tower</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>xxxxx</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>PY_VAR0</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>PY_VAR1</t>
+        </is>
+      </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X14" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="Y14" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>